<commit_message>
簡易実行メソッド Expect / ExpectReturn / ExpectThrown を追加する。(#3)
</commit_message>
<xml_diff>
--- a/FixtureBookTest/FixtureTest/FixtureBookTest.xlsx
+++ b/FixtureBookTest/FixtureTest/FixtureBookTest.xlsx
@@ -10,13 +10,15 @@
     <sheet name="FixtureBookTest" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Expect" sheetId="5" r:id="rId4"/>
+    <sheet name="ExpectThrown" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
   <si>
     <t>A. テストケース</t>
     <phoneticPr fontId="3"/>
@@ -208,6 +210,80 @@
   <si>
     <t>ValidateStorageの呼び出し時にはSetupメソッドの暗黙呼び出しはされないこと</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>E. 取得データ</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>A. テストケース</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>zzz</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ExpectおよびExpectResultのテスト</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Parameter1</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ghi</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>jkl</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Parameter2</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Parameter3</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Parameter4</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>ExpectThrownのテスト</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Message</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Validateで例外発生がテストできる</t>
+    <rPh sb="9" eb="11">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ハッセイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>xxx</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Exception</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
@@ -696,9 +772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E55"/>
+  <dimension ref="B2:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6"/>
   <cols>
@@ -713,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="3" customFormat="1">
+    <row r="4" spans="2:4">
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
@@ -723,19 +801,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="3" customFormat="1">
+    <row r="7" spans="2:4">
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:4" s="3" customFormat="1">
+    <row r="8" spans="2:4">
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="3" customFormat="1">
+    <row r="9" spans="2:4">
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
         <v>4</v>
@@ -890,34 +968,88 @@
       </c>
     </row>
     <row r="48" spans="2:4" s="6" customFormat="1"/>
-    <row r="49" spans="2:4" s="6" customFormat="1"/>
-    <row r="50" spans="2:4" s="2" customFormat="1">
+    <row r="49" spans="2:5" s="6" customFormat="1"/>
+    <row r="50" spans="2:5" s="2" customFormat="1">
       <c r="B50" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="2:4" s="6" customFormat="1">
+    <row r="51" spans="2:5" s="6" customFormat="1">
       <c r="C51" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="2:4" s="6" customFormat="1">
+    <row r="52" spans="2:5" s="6" customFormat="1">
       <c r="D52" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="2:4" s="6" customFormat="1">
+    <row r="53" spans="2:5" s="6" customFormat="1">
       <c r="D53" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="2:4" s="6" customFormat="1">
+    <row r="54" spans="2:5" s="6" customFormat="1">
       <c r="D54" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="2:4" s="6" customFormat="1"/>
+    <row r="55" spans="2:5" s="6" customFormat="1"/>
+    <row r="57" spans="2:5" s="1" customFormat="1">
+      <c r="B57" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="C59" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="13.8" customHeight="1"/>
+    <row r="61" spans="2:5" s="2" customFormat="1">
+      <c r="B61" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" s="6" customFormat="1">
+      <c r="C62" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="2:5" s="6" customFormat="1">
+      <c r="D63" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="2:5" s="6" customFormat="1">
+      <c r="D64" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="66" spans="3:5" s="6" customFormat="1">
+      <c r="C66" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="5"/>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="3:5" s="6" customFormat="1">
+      <c r="D67" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="3:5" s="6" customFormat="1">
+      <c r="D68" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -944,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="3" customFormat="1">
+    <row r="4" spans="2:4">
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
@@ -954,19 +1086,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="3" customFormat="1">
+    <row r="7" spans="2:4">
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:4" s="3" customFormat="1">
+    <row r="8" spans="2:4">
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="3" customFormat="1">
+    <row r="9" spans="2:4">
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
         <v>5</v>
@@ -977,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:4" s="3" customFormat="1">
+    <row r="14" spans="2:4">
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
@@ -987,19 +1119,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" s="3" customFormat="1">
+    <row r="17" spans="2:4">
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="2:4" s="3" customFormat="1">
+    <row r="18" spans="2:4">
       <c r="C18" s="6"/>
       <c r="D18" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:4" s="3" customFormat="1">
+    <row r="19" spans="2:4">
       <c r="C19" s="6"/>
       <c r="D19" s="8" t="s">
         <v>6</v>
@@ -1010,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:4" s="3" customFormat="1">
+    <row r="24" spans="2:4">
       <c r="C24" s="3" t="s">
         <v>12</v>
       </c>
@@ -1020,19 +1152,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:4" s="3" customFormat="1">
+    <row r="27" spans="2:4">
       <c r="C27" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="2:4" s="3" customFormat="1">
+    <row r="28" spans="2:4">
       <c r="C28" s="6"/>
       <c r="D28" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:4" s="3" customFormat="1">
+    <row r="29" spans="2:4">
       <c r="C29" s="6"/>
       <c r="D29" s="8" t="s">
         <v>9</v>
@@ -1063,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4" s="3" customFormat="1">
+    <row r="4" spans="2:4">
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1073,19 +1205,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="3" customFormat="1">
+    <row r="7" spans="2:4">
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:4" s="3" customFormat="1">
+    <row r="8" spans="2:4">
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" s="3" customFormat="1">
+    <row r="9" spans="2:4">
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
         <v>7</v>
@@ -1096,7 +1228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:4" s="3" customFormat="1">
+    <row r="14" spans="2:4">
       <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1106,19 +1238,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" s="3" customFormat="1">
+    <row r="17" spans="3:4">
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="3:4" s="3" customFormat="1">
+    <row r="18" spans="3:4">
       <c r="C18" s="6"/>
       <c r="D18" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="3:4" s="3" customFormat="1">
+    <row r="19" spans="3:4">
       <c r="C19" s="6"/>
       <c r="D19" s="8" t="s">
         <v>8</v>
@@ -1128,4 +1260,270 @@
   <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6"/>
+  <cols>
+    <col min="1" max="2" width="2.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" style="3" customWidth="1"/>
+    <col min="4" max="256" width="16.77734375" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" s="1" customFormat="1">
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" s="2" customFormat="1">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="C9" s="6"/>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="C12" s="6"/>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="C13" s="6"/>
+      <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="C17" s="6"/>
+      <c r="D17" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="C19" s="6"/>
+      <c r="D19" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="C20" s="6"/>
+      <c r="D20" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" s="2" customFormat="1">
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" s="6" customFormat="1">
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" s="6" customFormat="1">
+      <c r="D25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="2:5" s="6" customFormat="1">
+      <c r="D26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6"/>
+  <cols>
+    <col min="1" max="2" width="2.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="2.77734375" style="3" customWidth="1"/>
+    <col min="4" max="256" width="16.77734375" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" s="1" customFormat="1">
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="C4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" s="2" customFormat="1">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="C9" s="6"/>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="C12" s="6"/>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="C13" s="6"/>
+      <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="C15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="C17" s="6"/>
+      <c r="D17" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="C19" s="6"/>
+      <c r="D19" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="C20" s="6"/>
+      <c r="D20" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" s="2" customFormat="1">
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" s="6" customFormat="1">
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" s="6" customFormat="1">
+      <c r="D25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="2:5" s="6" customFormat="1">
+      <c r="D26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>